<commit_message>
adding sign in related files
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{30324CD0-07B3-4AE2-A027-80CB6D3F6794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="12300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="3" r:id="rId1"/>
@@ -13,19 +14,11 @@
     <sheet name="login_invalid" sheetId="6" r:id="rId4"/>
     <sheet name="TryEditorPage_Data" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:F21"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -163,8 +156,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,7 +229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -258,42 +251,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -597,244 +587,244 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="14" style="19" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="62.140625" style="19" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="19"/>
+    <col min="1" max="1" width="13.81640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="14" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.453125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="23.453125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="62.1796875" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="8">
         <v>12345</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="8">
         <v>12345</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="8" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="C6" r:id="rId7"/>
-    <hyperlink ref="B7" r:id="rId8"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -842,22 +832,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="8"/>
+    <col min="1" max="1" width="16.453125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -868,7 +858,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -885,25 +875,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="12.7109375" style="11"/>
+    <col min="1" max="1" width="21.81640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="12.7265625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75" customHeight="1">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
@@ -912,7 +902,7 @@
       </c>
       <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1">
+    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>23</v>
       </c>
@@ -943,17 +933,17 @@
       <c r="X2" s="13"/>
       <c r="Y2" s="13"/>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1">
+    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1">
+    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1">
+    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -964,25 +954,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" style="9" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" style="9"/>
-    <col min="4" max="4" width="32.140625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="12.7109375" style="9"/>
+    <col min="1" max="1" width="40.26953125" style="9" customWidth="1"/>
+    <col min="2" max="3" width="12.7265625" style="9"/>
+    <col min="4" max="4" width="32.1796875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="12.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -997,7 +987,7 @@
       </c>
       <c r="E1" s="10"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>22</v>
       </c>
@@ -1012,7 +1002,7 @@
       </c>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1013,7 @@
       </c>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>29</v>
       </c>
@@ -1036,7 +1026,7 @@
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>30</v>
       </c>
@@ -1049,7 +1039,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
@@ -1064,7 +1054,7 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>34</v>
       </c>
@@ -1079,14 +1069,14 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1099,22 +1089,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="14.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.54296875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1142,7 +1132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1156,7 +1146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1164,40 +1154,40 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="raj@123"/>
+    <hyperlink ref="B2" r:id="rId1" display="raj@123" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
updated added test data providers,excel data reader,try editor,updated base test,homepage,config,TestData.xlsxand testng.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -3,19 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{30324CD0-07B3-4AE2-A027-80CB6D3F6794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\myng\DSALGO231_TESTNG\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81337C63-4EE7-4A32-8FFA-8096B9E9AC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="20700" windowHeight="12300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="3" r:id="rId1"/>
-    <sheet name="Register_valid" sheetId="4" r:id="rId2"/>
-    <sheet name="login_valid" sheetId="5" r:id="rId3"/>
-    <sheet name="login_invalid" sheetId="6" r:id="rId4"/>
-    <sheet name="TryEditorPage_Data" sheetId="2" r:id="rId5"/>
+    <sheet name="TryEditorPage_Data" sheetId="7" r:id="rId2"/>
+    <sheet name="Register_valid" sheetId="4" r:id="rId3"/>
+    <sheet name="login_valid" sheetId="8" r:id="rId4"/>
+    <sheet name="login_invalid" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F21"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -229,39 +233,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -278,6 +259,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -341,7 +337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -393,7 +389,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -601,217 +597,217 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="14" style="8" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="23.453125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="62.1796875" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="8"/>
+    <col min="1" max="1" width="13.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="62.21875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="2">
         <v>12345</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="2">
         <v>12345</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -832,6 +828,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584727AF-A819-45C2-A603-9B60A0C845AA}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="raj@123" xr:uid="{6F409C04-D932-408F-A21F-2DF6F44B035D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -839,15 +909,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="23.54296875" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="8"/>
+    <col min="1" max="1" width="16.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -858,7 +928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -868,85 +938,6 @@
       <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:Y5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.81640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="27.26953125" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="12.7265625" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="12"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-    </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -954,242 +945,167 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECC020B-6629-44FF-BB53-F9375C75E35A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.26953125" style="9" customWidth="1"/>
-    <col min="2" max="3" width="12.7265625" style="9"/>
-    <col min="4" max="4" width="32.1796875" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="12.7265625" style="9"/>
+    <col min="1" max="1" width="40.21875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="12.77734375" style="3"/>
+    <col min="4" max="4" width="32.21875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="12.77734375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="10"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.54296875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="raj@123" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ExcelDataReader and excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\IdeaProjects\myng\DSALGO231_TESTNG\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSALGO231Testers_TestNg\DSALGO231_TESTNG\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D71D6F-1B79-43F8-AD3E-F782747B29D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F6289C-8657-4DA6-96AA-BB158337F425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="768" windowWidth="23040" windowHeight="11460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="3" r:id="rId1"/>
     <sheet name="Register_valid" sheetId="4" r:id="rId2"/>
-    <sheet name="login_valid" sheetId="8" r:id="rId3"/>
-    <sheet name="login_invalid" sheetId="6" r:id="rId4"/>
+    <sheet name="login_valid" sheetId="10" r:id="rId3"/>
+    <sheet name="login_invalid" sheetId="9" r:id="rId4"/>
     <sheet name="TryEditorPage_Data" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -197,24 +197,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFCCE5FF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -245,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -253,23 +241,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -621,13 +607,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -638,13 +624,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -655,13 +641,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -672,13 +658,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -689,13 +675,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -706,13 +692,13 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -723,13 +709,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -740,7 +726,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2">
@@ -757,13 +743,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -774,13 +760,13 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -791,13 +777,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -867,39 +853,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECC020B-6629-44FF-BB53-F9375C75E35A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC033930-A3B0-4496-B509-897558B914ED}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -909,120 +892,94 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DFEEEE-6400-44F1-9F5F-49E5C2C8A8F8}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="3"/>
-    <col min="3" max="3" width="34.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="12.77734375" style="3"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1033,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584727AF-A819-45C2-A603-9B60A0C845AA}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -1063,13 +1020,13 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1077,13 +1034,13 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1091,9 +1048,9 @@
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
committing registerpage and excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSALGO231Testers_TestNg\DSALGO231_TESTNG\src\test\resources\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F6289C-8657-4DA6-96AA-BB158337F425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="3" r:id="rId1"/>
@@ -19,9 +13,9 @@
     <sheet name="login_invalid" sheetId="9" r:id="rId4"/>
     <sheet name="TryEditorPage_Data" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -83,9 +77,6 @@
   </si>
   <si>
     <t>hj56</t>
-  </si>
-  <si>
-    <t>empty</t>
   </si>
   <si>
     <t>Password confirmation</t>
@@ -166,8 +157,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,7 +252,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -319,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -371,7 +362,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -565,102 +556,88 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="62.21875" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.77734375" style="2"/>
+    <col min="3" max="3" width="22.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="62.28515625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
@@ -668,30 +645,28 @@
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -702,13 +677,13 @@
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -719,13 +694,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -736,13 +711,13 @@
         <v>12345</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -753,13 +728,13 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -770,13 +745,13 @@
         <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -787,22 +762,22 @@
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="C6" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -810,41 +785,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.77734375" style="2"/>
+    <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -853,37 +828,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC033930-A3B0-4496-B509-897558B914ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -892,93 +867,93 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DFEEEE-6400-44F1-9F5F-49E5C2C8A8F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -987,22 +962,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584727AF-A819-45C2-A603-9B60A0C845AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +991,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1030,7 +1005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1044,7 +1019,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1054,7 +1029,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="raj@123" xr:uid="{6F409C04-D932-408F-A21F-2DF6F44B035D}"/>
+    <hyperlink ref="B2" r:id="rId1" display="raj@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated ds portal, home page ,try editor, and excel data reader
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSALGO231Testers_TestNg\DSALGO231_TESTNG\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B55743B-D551-48FC-9F55-2A0A399DA64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register_invalid" sheetId="3" r:id="rId1"/>
@@ -14,8 +20,8 @@
     <sheet name="TryEditorPage_Data" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
-  <si>
-    <t>ScenarioName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
   <si>
     <t>Code</t>
   </si>
@@ -37,9 +40,6 @@
     <t>Message</t>
   </si>
   <si>
-    <t>Valid Code</t>
-  </si>
-  <si>
     <t>print("hello dsalgo231testers")</t>
   </si>
   <si>
@@ -49,9 +49,6 @@
     <t>hello dsalgo231testers</t>
   </si>
   <si>
-    <t>Invalid Code</t>
-  </si>
-  <si>
     <t>print(invalid code)</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
   </si>
   <si>
     <t>SyntaxError: bad input on line 1</t>
-  </si>
-  <si>
-    <t>No Code</t>
   </si>
   <si>
     <t>hjkl@45</t>
@@ -157,8 +151,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,21 +232,21 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -556,153 +550,153 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="62.28515625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="2"/>
+    <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="62.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>12345</v>
@@ -711,73 +705,73 @@
         <v>12345</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="C6" r:id="rId7"/>
-    <hyperlink ref="B7" r:id="rId8"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -785,41 +779,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="16.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -828,37 +822,37 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -867,93 +861,93 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -962,22 +956,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -987,49 +980,37 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="4"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="raj@123"/>
+    <hyperlink ref="A2" r:id="rId1" display="raj@123" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>